<commit_message>
update symbol and buckets
add the estimation of # of stroke for each equation
</commit_message>
<xml_diff>
--- a/Symbols - Buckets/Symbols & Buckets.xlsx
+++ b/Symbols - Buckets/Symbols & Buckets.xlsx
@@ -1,17 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
   <workbookPr filterPrivacy="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chensi/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Symbol Bucket" sheetId="1" r:id="rId1"/>
+    <sheet name="stroke#" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -19,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
   <si>
     <t>+</t>
   </si>
@@ -136,12 +148,42 @@
   </si>
   <si>
     <t>+ -</t>
+  </si>
+  <si>
+    <t>equation</t>
+  </si>
+  <si>
+    <t># of stroke before combine</t>
+  </si>
+  <si>
+    <t># of strokes after combine</t>
+  </si>
+  <si>
+    <t># of stroke before combination of division mark, equal mark and i</t>
+  </si>
+  <si>
+    <t># of strokes after combination of division mark, equal mark and i</t>
+  </si>
+  <si>
+    <t># of strokes of combined</t>
+  </si>
+  <si>
+    <t># of strokes of combined symbol like sin as sin based on combination of division, equal and i</t>
+  </si>
+  <si>
+    <t>...</t>
+  </si>
+  <si>
+    <t>pattern can be separated or not</t>
+  </si>
+  <si>
+    <t>pattern must be combined</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -151,15 +193,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -167,16 +215,106 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -189,6 +327,138 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>651814</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>34700</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="224666" cy="172227"/>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5347237" y="1573010"/>
+              <a:ext cx="224666" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a14:m>
+                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                  <m:oMathParaPr>
+                    <m:jc m:val="centerGroup"/>
+                  </m:oMathParaPr>
+                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
+                    <m:acc>
+                      <m:accPr>
+                        <m:chr m:val="̅"/>
+                        <m:ctrlPr>
+                          <a:rPr lang="en-US" sz="1100" i="1">
+                            <a:latin typeface="Cambria Math" charset="0"/>
+                          </a:rPr>
+                        </m:ctrlPr>
+                      </m:accPr>
+                      <m:e>
+                        <m:r>
+                          <a:rPr lang="en-US" sz="1100" b="0" i="1">
+                            <a:latin typeface="Cambria Math" charset="0"/>
+                          </a:rPr>
+                          <m:t>𝑥</m:t>
+                        </m:r>
+                      </m:e>
+                    </m:acc>
+                  </m:oMath>
+                </m:oMathPara>
+              </a14:m>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="2" name="TextBox 1"/>
+            <xdr:cNvSpPr txBox="1"/>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5347237" y="1573010"/>
+              <a:ext cx="224666" cy="172227"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+          </xdr:spPr>
+          <xdr:style>
+            <a:lnRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:lnRef>
+            <a:fillRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:fillRef>
+            <a:effectRef idx="0">
+              <a:scrgbClr r="0" g="0" b="0"/>
+            </a:effectRef>
+            <a:fontRef idx="minor">
+              <a:schemeClr val="tx1"/>
+            </a:fontRef>
+          </xdr:style>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-US" sz="1100" b="0" i="0">
+                  <a:latin typeface="Cambria Math" charset="0"/>
+                </a:rPr>
+                <a:t>𝑥 ̅</a:t>
+              </a:r>
+              <a:endParaRPr lang="en-US" sz="1100"/>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -454,15 +724,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G37"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView zoomScale="142" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="13.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>0</v>
       </c>
@@ -473,71 +746,138 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I2" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4"/>
+      <c r="M2" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="3"/>
+      <c r="O2" s="4"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J3" s="6"/>
+      <c r="K3" s="7"/>
+      <c r="M3" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="N3" s="6"/>
+      <c r="O3" s="7"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="C4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="6"/>
+      <c r="K4" s="7"/>
+      <c r="M4" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="N4" s="6"/>
+      <c r="O4" s="7"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="C5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I5" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="M5" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="7"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>6</v>
       </c>
       <c r="C6">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" s="6"/>
+      <c r="K6" s="7"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="7"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>7</v>
       </c>
       <c r="C7" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="6"/>
+      <c r="K7" s="7"/>
+      <c r="M7" s="5"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="7"/>
+    </row>
+    <row r="8" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
       <c r="C8" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="J8" s="6"/>
+      <c r="K8" s="7"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="10"/>
+    </row>
+    <row r="9" spans="1:15" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="I9" s="8"/>
+      <c r="J9" s="9"/>
+      <c r="K9" s="10"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>10</v>
       </c>
@@ -545,7 +885,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -553,7 +893,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
@@ -561,7 +901,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>13</v>
       </c>
@@ -569,7 +909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>14</v>
       </c>
@@ -577,7 +917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>15</v>
       </c>
@@ -585,7 +925,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>16</v>
       </c>
@@ -593,7 +933,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>17</v>
       </c>
@@ -601,7 +941,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>18</v>
       </c>
@@ -609,7 +949,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>19</v>
       </c>
@@ -617,7 +957,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>20</v>
       </c>
@@ -625,7 +965,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>21</v>
       </c>
@@ -639,7 +979,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>22</v>
       </c>
@@ -647,12 +987,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>23</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>24</v>
       </c>
@@ -660,7 +1000,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>25</v>
       </c>
@@ -668,7 +1008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>26</v>
       </c>
@@ -679,7 +1019,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>27</v>
       </c>
@@ -690,7 +1030,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>28</v>
       </c>
@@ -698,7 +1038,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>29</v>
       </c>
@@ -706,7 +1046,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>30</v>
       </c>
@@ -717,7 +1057,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>31</v>
       </c>
@@ -728,7 +1068,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>32</v>
       </c>
@@ -736,7 +1076,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>33</v>
       </c>
@@ -747,7 +1087,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>34</v>
       </c>
@@ -758,7 +1098,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>35</v>
       </c>
@@ -766,7 +1106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>37</v>
       </c>
@@ -774,7 +1114,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>38</v>
       </c>
@@ -785,5 +1125,554 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D39"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScale="167" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="7"/>
+    </row>
+    <row r="3" spans="1:4" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>11</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>16</v>
+      </c>
+      <c r="C11">
+        <v>15</v>
+      </c>
+      <c r="D11">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>9</v>
+      </c>
+      <c r="D14">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+      <c r="D15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>17</v>
+      </c>
+      <c r="C16">
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>10</v>
+      </c>
+      <c r="D17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>9</v>
+      </c>
+      <c r="C18">
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>14</v>
+      </c>
+      <c r="C19">
+        <v>13</v>
+      </c>
+      <c r="D19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>25</v>
+      </c>
+      <c r="C20">
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>13</v>
+      </c>
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>11</v>
+      </c>
+      <c r="C23">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>17</v>
+      </c>
+      <c r="C25">
+        <v>15</v>
+      </c>
+      <c r="D25">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>21</v>
+      </c>
+      <c r="C26">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27">
+        <v>20</v>
+      </c>
+      <c r="D27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>6</v>
+      </c>
+      <c r="C28">
+        <v>6</v>
+      </c>
+      <c r="D28">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>25</v>
+      </c>
+      <c r="B29">
+        <v>12</v>
+      </c>
+      <c r="C29">
+        <v>11</v>
+      </c>
+      <c r="D29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>26</v>
+      </c>
+      <c r="B30">
+        <v>16</v>
+      </c>
+      <c r="C30">
+        <v>15</v>
+      </c>
+      <c r="D30">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>27</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+      <c r="C31">
+        <v>11</v>
+      </c>
+      <c r="D31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>28</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32">
+        <v>6</v>
+      </c>
+      <c r="D32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>29</v>
+      </c>
+      <c r="B33">
+        <v>12</v>
+      </c>
+      <c r="C33">
+        <v>11</v>
+      </c>
+      <c r="D33">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>30</v>
+      </c>
+      <c r="B34">
+        <v>7</v>
+      </c>
+      <c r="C34">
+        <v>6</v>
+      </c>
+      <c r="D34">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>31</v>
+      </c>
+      <c r="B35">
+        <v>12</v>
+      </c>
+      <c r="C35">
+        <v>11</v>
+      </c>
+      <c r="D35">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>32</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37">
+        <v>11</v>
+      </c>
+      <c r="D37">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>34</v>
+      </c>
+      <c r="B38">
+        <v>14</v>
+      </c>
+      <c r="C38">
+        <v>13</v>
+      </c>
+      <c r="D38">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39">
+        <v>35</v>
+      </c>
+      <c r="B39">
+        <v>15</v>
+      </c>
+      <c r="C39">
+        <v>14</v>
+      </c>
+      <c r="D39">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>